<commit_message>
Atualização da aula de Tratativas de Exceções na UiPath.
</commit_message>
<xml_diff>
--- a/Realizar Cálculos.xlsx
+++ b/Realizar Cálculos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo\Documents\UiPath\RPA-Aula-TratativasExcecoes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E1A15E-E892-4050-80DC-82D2E87BD49D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB41B17-52C8-4A74-9129-FD8AD33DDF98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4530" windowWidth="8205" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cálculos" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="17">
   <si>
     <t>Número A</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>f27</t>
+  </si>
+  <si>
+    <t>ERRO</t>
   </si>
 </sst>
 </file>
@@ -460,6 +463,9 @@
       <c r="C2" s="2">
         <v>30</v>
       </c>
+      <c r="D2" s="2">
+        <v>31</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -471,6 +477,9 @@
       <c r="C3" s="2">
         <v>29</v>
       </c>
+      <c r="D3" s="2">
+        <v>-27</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -482,6 +491,9 @@
       <c r="C4" s="2">
         <v>28</v>
       </c>
+      <c r="D4" s="2">
+        <v>84</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -493,7 +505,9 @@
       <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -504,6 +518,9 @@
       </c>
       <c r="C6" s="2">
         <v>26</v>
+      </c>
+      <c r="D6" s="2">
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -516,6 +533,9 @@
       <c r="C7" s="2">
         <v>25</v>
       </c>
+      <c r="D7" s="2">
+        <v>-19</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -527,6 +547,9 @@
       <c r="C8" s="2">
         <v>24</v>
       </c>
+      <c r="D8" s="2">
+        <v>168</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -538,6 +561,9 @@
       <c r="C9" s="2">
         <v>23</v>
       </c>
+      <c r="D9" s="2">
+        <v>0.34782608695652201</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -549,6 +575,9 @@
       <c r="C10" s="2">
         <v>22</v>
       </c>
+      <c r="D10" s="2">
+        <v>31</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -560,6 +589,9 @@
       <c r="C11" s="2">
         <v>21</v>
       </c>
+      <c r="D11" s="2">
+        <v>-11</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -571,7 +603,9 @@
       <c r="C12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -583,6 +617,9 @@
       <c r="C13" s="2">
         <v>19</v>
       </c>
+      <c r="D13" s="2">
+        <v>0.63157894736842102</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -594,6 +631,9 @@
       <c r="C14" s="2">
         <v>18</v>
       </c>
+      <c r="D14" s="2">
+        <v>31</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
@@ -605,6 +645,9 @@
       <c r="C15" s="2">
         <v>17</v>
       </c>
+      <c r="D15" s="2">
+        <v>-3</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
@@ -616,6 +659,9 @@
       <c r="C16" s="2">
         <v>16</v>
       </c>
+      <c r="D16" s="2">
+        <v>240</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
@@ -627,7 +673,9 @@
       <c r="C17" s="3">
         <v>15</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
@@ -639,6 +687,9 @@
       <c r="C18" s="2">
         <v>14</v>
       </c>
+      <c r="D18" s="2">
+        <v>31</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
@@ -650,6 +701,9 @@
       <c r="C19" s="2">
         <v>13</v>
       </c>
+      <c r="D19" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
@@ -661,6 +715,9 @@
       <c r="C20" s="2">
         <v>12</v>
       </c>
+      <c r="D20" s="2">
+        <v>228</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
@@ -672,6 +729,9 @@
       <c r="C21" s="2">
         <v>11</v>
       </c>
+      <c r="D21" s="2">
+        <v>1.8181818181818199</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
@@ -683,7 +743,9 @@
       <c r="C22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
@@ -695,6 +757,9 @@
       <c r="C23" s="2">
         <v>9</v>
       </c>
+      <c r="D23" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
@@ -706,6 +771,9 @@
       <c r="C24" s="2">
         <v>8</v>
       </c>
+      <c r="D24" s="2">
+        <v>184</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
@@ -717,6 +785,9 @@
       <c r="C25" s="2">
         <v>7</v>
       </c>
+      <c r="D25" s="2">
+        <v>3.4285714285714302</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
@@ -728,7 +799,9 @@
       <c r="C26" s="3">
         <v>6</v>
       </c>
-      <c r="D26" s="3"/>
+      <c r="D26" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
@@ -740,6 +813,9 @@
       <c r="C27" s="2">
         <v>5</v>
       </c>
+      <c r="D27" s="2">
+        <v>21</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
@@ -751,6 +827,9 @@
       <c r="C28" s="2">
         <v>4</v>
       </c>
+      <c r="D28" s="2">
+        <v>108</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
@@ -762,6 +841,9 @@
       <c r="C29" s="2">
         <v>3</v>
       </c>
+      <c r="D29" s="2">
+        <v>9.3333333333333304</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
@@ -773,6 +855,9 @@
       <c r="C30" s="2">
         <v>2</v>
       </c>
+      <c r="D30" s="2">
+        <v>31</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
@@ -784,7 +869,9 @@
       <c r="C31" s="3">
         <v>1</v>
       </c>
-      <c r="D31" s="3"/>
+      <c r="D31" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>